<commit_message>
Some minor changes to feat wordings
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Feats/Feats.xlsx
+++ b/CoreRulebook/Data/Feats/Feats.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$106</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$91</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$105</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$93</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$90</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="250">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">\imp{Alteration} (\fiveCape{})</t>
   </si>
   <si>
-    <t xml:space="preserve">As an exceptionally powerful Thaumaturge, you have learned to shift your shape into that of an animal. By expending a \imp{Fortitude} point, you may instantly assume the physical attributes of your `spirit animal’. This animal is (usually) the same as your \imp{Patronus} and can only be changed if your undergo a profound change on a spiritual level. 
+    <t xml:space="preserve">As an exceptionally powerful Thaumaturge, you have learned to shift your shape into that of an animal. By expending a \imp{Fortitude} point, you may instantly assume the physical attributes of your `spirit animal’. This animal is (usually) the same as your \imp{Patronus} and can only be changed if your undergo a profound change on a spiritual level. Whilst in this form, you retain your mental state, but all your physical statistics and abilities are replaced by those of the form you take. 
 You may choose to revert back to your human form at any time, and you do so automatically if you are reduced to a \imp{Critical Condition} whilst in bestial form. </t>
   </si>
   <si>
@@ -58,16 +58,10 @@
     <t xml:space="preserve">When a target attempts to block your attacks, their armour takes an additional level of \imp{Drain}: a \imp{full-round block} incurs one level of drain, and \imp{quickblocking} incurs two levels. </t>
   </si>
   <si>
-    <t xml:space="preserve">Attuned Attacks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When fighting unarmed, or with a non-magical weapon, you can channel your very life-force into your attacks. Such attacks deal an additional level harm, and bypass any resistance to physical attacks. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Crash Course</t>
   </si>
   <si>
-    <t xml:space="preserve">You study a crash course in a selection of 10 abilities you previously had no skill in, giving you a basic level of knowledge. Choose up to 10 \imp{Abilities} with a \emptyCape{} rating, and gain 1 dot in each of them. If, when you take this ability, it costs more than 9 dots, pay only 9 dots. </t>
+    <t xml:space="preserve">You study a crash course in a selection of 10 abilities you previously had no skill in, giving you a basic level of knowledge. Choose up to 10 \imp{Abilities} with a \emptyCape{} rating, and gain 1 dot in each of them. If, when you take this ability, it would cost more than 9 dots, pay only 9 dots. </t>
   </si>
   <si>
     <t xml:space="preserve">Elemental Attunement</t>
@@ -76,13 +70,13 @@
     <t xml:space="preserve">\imp{Elemental} (\threeCape{})</t>
   </si>
   <si>
-    <t xml:space="preserve">You feel a particular affinity for one of the elements (Fire, Water, Ice, Earth, Air, Lightning, etc.) deep within your bones. When casting a spell to manipulate, create or otherwise effect your chosen element, you gain +1d. You also gain +1d to any check to resist damage caused by your element. </t>
+    <t xml:space="preserve">You feel a particular affinity for one of the elements (Fire, Water, Ice, Earth, Air, Lightning, etc.) deep within your bones. When casting a spell to manipulate, create or otherwise effect your chosen element, you gain +1d. You also gain +1d to any check to \imp{resist }damage caused by your element. </t>
   </si>
   <si>
     <t xml:space="preserve">First Aid</t>
   </si>
   <si>
-    <t xml:space="preserve">You know the basics of helping others and mainting life. Whenever a being falls into the \imp{critical condition} status within 3m of you, you may expend a \imp{Fortitude} point to allow them to perform emergency care. Perform a DV 6 \imp{Insight (Kindness)} check, and heal them by an amount equal to the number of successes. If you have a \imp{First Aid Kit}, you may expend that rather than a \imp{Fortitude} point.</t>
+    <t xml:space="preserve">You know the basics of helping others and mainting life. Whenever a being falls into the \imp{critical condition} status within 3m of you, you may expend a \imp{Fortitude} point to allow them to perform emergency care. Perform a DV 8 \imp{Insight (Kindness)} check, and heal them by an amount equal to the number of successes, removing the \imp{Critical Condition} status. If you have a \imp{First Aid Kit}, you may expend that rather than a \imp{Fortitude} point.</t>
   </si>
   <si>
     <t xml:space="preserve">Helping Hand</t>
@@ -130,7 +124,7 @@
     <t xml:space="preserve">Kinship (\twoCape)</t>
   </si>
   <si>
-    <t xml:space="preserve">You have an animal ally which is eternally loyal and devoted to you, and can carry out simple tasks: a `familiar’. This familiar is a well trained pet and will follow simple orders, though they cannot communicate back, though you maintain a weak psychic link allowing you to know their current physical condition. The most common animals are owls, ravens, cats, rats and toads, though you may ask your GM for a different choice. </t>
+    <t xml:space="preserve">You have an animal ally which is eternally loyal and devoted to you, and can carry out simple tasks: a `familiar’. This familiar is a well trained pet and will follow simple orders, though they cannot communicate back. You maintain a weak psychic link allowing you to know their current physical and emotional condition. The most common animals are owls, ravens, cats, rats and toads, though you may ask your GM for a different choice. </t>
   </si>
   <si>
     <t xml:space="preserve">Martial Arts</t>
@@ -139,7 +133,7 @@
     <t xml:space="preserve">Brawl (\threeCape)</t>
   </si>
   <si>
-    <t xml:space="preserve">You are a master of unarmed combat, making your hands into lethal weapons. Unarmed strikes now deal an additional level of damage (1 + \# Successes), with a reduced DV of 4. </t>
+    <t xml:space="preserve">You are a master of unarmed combat, making your hands into lethal weapons. Unarmed strikes now deal an additional level of damage (1 + \# Successes), with a reduced DV of 4. In addition, before making an attack roll, you may expend a \imp{Fortitude} point to automatically roll all your \imp{Brawl} dice as successes. </t>
   </si>
   <si>
     <t xml:space="preserve">Moving Target</t>
@@ -160,7 +154,7 @@
     <t xml:space="preserve">Parry Master</t>
   </si>
   <si>
-    <t xml:space="preserve">Carrying a melee weapon grants a +2 to your base \imp{block} bonus. </t>
+    <t xml:space="preserve">Carrying a melee weapon grants a +2 to your base \imp{block} bonus, in addition, if you \imp{Block} an incoming melee attack to a power of \imp{zero}, you may expend a \imp{fortitude} point to \imp{disarm} your attacker.</t>
   </si>
   <si>
     <t xml:space="preserve">Psychic Awareness</t>
@@ -169,7 +163,7 @@
     <t xml:space="preserve">\imp{Kindness} (\threeCape{}) </t>
   </si>
   <si>
-    <t xml:space="preserve">Your mind is especially attuned to those of others, and you can naturally sense the shift induced when a psychic power alters or interacts with minds. Whenever a psychic effect such as mind reading, memory modification, or magic which alters emotions and allegiances is used on a target within 5m of you, you are automatically aware of this, though you are not aware of the source. </t>
+    <t xml:space="preserve">Your mind is especially attuned to those of others, and you can naturally sense the shift induced when a psychic power alters or interacts with minds. Whenever a psychic effect such as mind reading, memory modification, or magic which alters emotions and allegiances is used on a target within 5m of you, you are instantly aware of this – you may expend a \imp{fortitude} point to learn the target of the spell, as well as the caster and the intent of the spell. </t>
   </si>
   <si>
     <t xml:space="preserve">Ritualist</t>
@@ -190,13 +184,13 @@
     <t xml:space="preserve">Signature Spell</t>
   </si>
   <si>
-    <t xml:space="preserve">You have a spell which is considered your `signature move’, chosen when you take this feat. When casting this spell, you gain one additional auto-success. You may change your `signature spell’ only with GM consent that your old choice no longer represents your character’s go-to move. </t>
+    <t xml:space="preserve">You have a spell which is considered your `signature move’, chosen when you take this feat. When casting this spell, \imp{catastrophes} are counted as normal failures. You may change your `signature spell’ only with GM consent that your old choice no longer represents your character’s go-to move. </t>
   </si>
   <si>
     <t xml:space="preserve">Silent Casting</t>
   </si>
   <si>
-    <t xml:space="preserve">You do not need to perform the verbal component of a spellcasting action. Efforts to silence you do not impact your spellcasting efforts, and reactions to your spells take a 1d penalty. </t>
+    <t xml:space="preserve">You do not need to perform the verbal component of a spellcasting action. Efforts to silence you do not impact your spellcasting efforts, and the lack of an alerting incantation means efforts to \imp{Resist} your spells take a 1d penalty. </t>
   </si>
   <si>
     <t xml:space="preserve">Wandless Casting</t>
@@ -217,7 +211,7 @@
     <t xml:space="preserve">Defensive Gadgets</t>
   </si>
   <si>
-    <t xml:space="preserve">At the end of every \imp{Long Rest}, you conceal a number of defensive doohickeys on your sleeve equal to your \imp{Danger} rating. You may expend one of these devices as an instantaneous action to ignore all effects of \imp{Drain} on a single \imp{Resist} roll. </t>
+    <t xml:space="preserve">At the end of every \imp{Long Rest}, you conceal a number of defensive doohickeys on your sleeve equal to your \imp{Danger} rating. You may expend one of these devices as an instantaneous action to gain the maximum number of successes on a single \imp{Resist} roll. </t>
   </si>
   <si>
     <t xml:space="preserve">Expert Enchanter</t>
@@ -245,7 +239,7 @@
     <t xml:space="preserve">Discerning Eyes</t>
   </si>
   <si>
-    <t xml:space="preserve">At the end of every \imp{Long Rest}, roll a DV 7 check using only your \imp{Analyse} pool (min 1 success). You may expend one of these successes as an instantaneous action to learn about a target as if you had cast the \imp{Identify} spell at \levelOne{} level (though this does not count as a \imp{spellcasting} effort, and cannot be percieved by others). You may increase the level of the effect by expending additional successes. </t>
+    <t xml:space="preserve">At the end of every \imp{Long Rest}, roll a DV 7 check using only your \imp{Analyse} pool (min 1 success). You may expend one of these successes as an instantaneous action to learn about a target as if you had cast the \imp{Identify} spell at \levelThree{} level (though this does not count as a \imp{spellcasting} effort, and cannot be percieved by others). You may increase the level of the effect by expending additional successes. </t>
   </si>
   <si>
     <t xml:space="preserve">Idiosyncrasies</t>
@@ -316,7 +310,7 @@
     <t xml:space="preserve">Deductive Senses</t>
   </si>
   <si>
-    <t xml:space="preserve">Your logical mind allows you to keep track of hidden foes. Whenever a creature that you can see goes invisible, or otherwise becomes undetectable to normal senses, perform a DV 8 \imp{Insight (Intuition)} check. For every success, you remain aware of the position of that creature for an additional \imp{Combat Cycle}, and do not treat it as invisible. </t>
+    <t xml:space="preserve">Your logical mind allows you to keep track of hidden foes. Whenever a creature that you can see goes invisible, or otherwise becomes undetectable to normal senses, perform a DV 8 \imp{Insight (Intuition)} check as an instantaneous action. For every success, you remain aware of the position of that creature for an additional \imp{Combat Cycle}, and do not treat it as invisible. </t>
   </si>
   <si>
     <t xml:space="preserve">Familiar Terrain</t>
@@ -340,7 +334,7 @@
     <t xml:space="preserve">Lie Detector</t>
   </si>
   <si>
-    <t xml:space="preserve">You can automatically detect when someone is lying to you by telling you deliberate falsehoods</t>
+    <t xml:space="preserve">You can automatically detect when someone is lying to you by telling you deliberate falsehoods. You may expend a \imp{Fortitude} point to get a glimpse at what they are hiding or lying about. </t>
   </si>
   <si>
     <t xml:space="preserve">Mental Training</t>
@@ -754,7 +748,7 @@
     <t xml:space="preserve">Alien Thoughts</t>
   </si>
   <si>
-    <t xml:space="preserve">Through some weird means you have attuned your mind to a different way of thinking, making it harder to infiltrate your mind. You are considered \imp{Resistant} to psychic damage, and effects to alter your mind have a DV two higher than normal. </t>
+    <t xml:space="preserve">Through some weird means, or simply deep meditation, you have attuned your mind to a different way of thinking, making it harder to infiltrate your mind. You are considered \imp{Resistant} to psychic damage, and effects to alter your mind have a DV two higher than normal. </t>
   </si>
   <si>
     <t xml:space="preserve">Open Mind</t>
@@ -913,10 +907,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A118" activeCellId="0" sqref="A118"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -942,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -961,7 +955,7 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">IF(NOT(E2=""),COUNTIF(B:B,E2),"")</f>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,7 +977,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1002,15 +996,18 @@
         <v/>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="false">IF(NOT(B5=B4),B5,"")</f>
@@ -1021,16 +1018,13 @@
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1043,7 +1037,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>17</v>
       </c>
@@ -1062,7 +1056,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
@@ -1081,7 +1075,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1094,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1113,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>25</v>
       </c>
@@ -1138,7 +1132,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>27</v>
       </c>
@@ -1157,15 +1151,18 @@
         <v/>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" s="0" t="str">
         <f aca="false">IF(NOT(B13=B12),B13,"")</f>
@@ -1176,18 +1173,18 @@
         <v/>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="0" t="str">
         <f aca="false">IF(NOT(B14=B13),B14,"")</f>
@@ -1200,13 +1197,10 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
@@ -1227,8 +1221,11 @@
       <c r="B16" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C16" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" s="0" t="str">
         <f aca="false">IF(NOT(B16=B15),B16,"")</f>
@@ -1239,16 +1236,13 @@
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1261,15 +1255,18 @@
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C18" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="false">IF(NOT(B18=B17),B18,"")</f>
@@ -1280,18 +1277,18 @@
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="0" t="str">
         <f aca="false">IF(NOT(B19=B18),B19,"")</f>
@@ -1302,16 +1299,13 @@
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
@@ -1324,7 +1318,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>50</v>
       </c>
@@ -1343,7 +1337,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>52</v>
       </c>
@@ -1362,13 +1356,16 @@
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C23" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>55</v>
       </c>
@@ -1381,53 +1378,50 @@
         <v/>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E24" s="0" t="str">
         <f aca="false">IF(NOT(B24=B23),B24,"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="0" t="str">
+        <v>Artificer</v>
+      </c>
+      <c r="F24" s="0" t="n">
         <f aca="false">IF(NOT(E24=""),COUNTIF(B:B,E24),"")</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="0" t="str">
         <f aca="false">IF(NOT(B25=B24),B25,"")</f>
-        <v>Artificer</v>
-      </c>
-      <c r="F25" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F25" s="0" t="str">
         <f aca="false">IF(NOT(E25=""),COUNTIF(B:B,E25),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>62</v>
@@ -1441,12 +1435,12 @@
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>64</v>
@@ -1460,12 +1454,12 @@
         <v/>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>66</v>
@@ -1484,7 +1478,7 @@
         <v>67</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>68</v>
@@ -1498,15 +1492,23 @@
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>69</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="E30" s="0" t="str">
+        <f aca="false">IF(NOT(B30=B29),B30,"")</f>
+        <v/>
+      </c>
+      <c r="F30" s="0" t="str">
+        <f aca="false">IF(NOT(E30=""),COUNTIF(B:B,E30),"")</f>
+        <v/>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,13 +1516,13 @@
         <v>71</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E31" s="0" t="str">
-        <f aca="false">IF(NOT(B31=B29),B31,"")</f>
+        <f aca="false">IF(NOT(B31=B30),B31,"")</f>
         <v/>
       </c>
       <c r="F31" s="0" t="str">
@@ -1528,15 +1530,23 @@
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>73</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="E32" s="0" t="str">
+        <f aca="false">IF(NOT(B32=B31),B32,"")</f>
+        <v/>
+      </c>
+      <c r="F32" s="0" t="str">
+        <f aca="false">IF(NOT(E32=""),COUNTIF(B:B,E32),"")</f>
+        <v/>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,13 +1554,13 @@
         <v>75</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E33" s="0" t="str">
-        <f aca="false">IF(NOT(B33=B31),B33,"")</f>
+        <f aca="false">IF(NOT(B33=B32),B33,"")</f>
         <v/>
       </c>
       <c r="F33" s="0" t="str">
@@ -1558,12 +1568,12 @@
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>78</v>
@@ -1577,15 +1587,23 @@
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>79</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>80</v>
+      </c>
+      <c r="E35" s="0" t="str">
+        <f aca="false">IF(NOT(B35=B34),B35,"")</f>
+        <v/>
+      </c>
+      <c r="F35" s="0" t="str">
+        <f aca="false">IF(NOT(E35=""),COUNTIF(B:B,E35),"")</f>
+        <v/>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,45 +1611,45 @@
         <v>81</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="0" t="str">
+        <f aca="false">IF(NOT(B36=B35),B36,"")</f>
+        <v>Auror</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">IF(NOT(E36=""),COUNTIF(B:B,E36),"")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="E36" s="0" t="str">
-        <f aca="false">IF(NOT(B36=B34),B36,"")</f>
-        <v/>
-      </c>
-      <c r="F36" s="0" t="str">
-        <f aca="false">IF(NOT(E36=""),COUNTIF(B:B,E36),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>84</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E37" s="0" t="str">
         <f aca="false">IF(NOT(B37=B36),B37,"")</f>
-        <v>Auror</v>
-      </c>
-      <c r="F37" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F37" s="0" t="str">
         <f aca="false">IF(NOT(E37=""),COUNTIF(B:B,E37),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>86</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>87</v>
@@ -1645,14 +1663,14 @@
         <v/>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E39" s="0" t="str">
@@ -1664,14 +1682,14 @@
         <v/>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>90</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E40" s="0" t="str">
@@ -1683,14 +1701,14 @@
         <v/>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>92</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E41" s="0" t="str">
@@ -1707,7 +1725,7 @@
         <v>94</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>95</v>
@@ -1721,14 +1739,14 @@
         <v/>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>96</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E43" s="0" t="str">
@@ -1740,14 +1758,14 @@
         <v/>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>98</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>99</v>
       </c>
       <c r="E44" s="0" t="str">
@@ -1759,14 +1777,14 @@
         <v/>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>100</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E45" s="0" t="str">
@@ -1778,14 +1796,14 @@
         <v/>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>102</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>103</v>
       </c>
       <c r="E46" s="0" t="str">
@@ -1797,12 +1815,12 @@
         <v/>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>104</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>105</v>
@@ -1816,42 +1834,42 @@
         <v/>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>106</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="false">IF(NOT(B48=B47),B48,"")</f>
-        <v/>
-      </c>
-      <c r="F48" s="0" t="str">
+        <v>Druid</v>
+      </c>
+      <c r="F48" s="0" t="n">
         <f aca="false">IF(NOT(E48=""),COUNTIF(B:B,E48),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E49" s="0" t="str">
         <f aca="false">IF(NOT(B49=B48),B49,"")</f>
-        <v>Druid</v>
-      </c>
-      <c r="F49" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F49" s="0" t="str">
         <f aca="false">IF(NOT(E49=""),COUNTIF(B:B,E49),"")</f>
-        <v>11</v>
+        <v/>
       </c>
     </row>
     <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,7 +1877,7 @@
         <v>111</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>112</v>
@@ -1873,29 +1891,37 @@
         <v/>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>113</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="0" t="str">
+        <f aca="false">IF(NOT(B51=B50),B51,"")</f>
+        <v/>
+      </c>
+      <c r="F51" s="0" t="str">
+        <f aca="false">IF(NOT(E51=""),COUNTIF(B:B,E51),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>115</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E52" s="0" t="str">
-        <f aca="false">IF(NOT(B52=B50),B52,"")</f>
+        <f aca="false">IF(NOT(B52=B51),B52,"")</f>
         <v/>
       </c>
       <c r="F52" s="0" t="str">
@@ -1903,29 +1929,37 @@
         <v/>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>117</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="0" t="str">
+        <f aca="false">IF(NOT(B53=B52),B53,"")</f>
+        <v/>
+      </c>
+      <c r="F53" s="0" t="str">
+        <f aca="false">IF(NOT(E53=""),COUNTIF(B:B,E53),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E54" s="0" t="str">
-        <f aca="false">IF(NOT(B54=B52),B54,"")</f>
+        <f aca="false">IF(NOT(B54=B53),B54,"")</f>
         <v/>
       </c>
       <c r="F54" s="0" t="str">
@@ -1933,29 +1967,37 @@
         <v/>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>121</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="0" t="str">
+        <f aca="false">IF(NOT(B55=B54),B55,"")</f>
+        <v/>
+      </c>
+      <c r="F55" s="0" t="str">
+        <f aca="false">IF(NOT(E55=""),COUNTIF(B:B,E55),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>123</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E56" s="0" t="str">
-        <f aca="false">IF(NOT(B56=B54),B56,"")</f>
+        <f aca="false">IF(NOT(B56=B55),B56,"")</f>
         <v/>
       </c>
       <c r="F56" s="0" t="str">
@@ -1963,29 +2005,37 @@
         <v/>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>125</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="0" t="str">
+        <f aca="false">IF(NOT(B57=B56),B57,"")</f>
+        <v/>
+      </c>
+      <c r="F57" s="0" t="str">
+        <f aca="false">IF(NOT(E57=""),COUNTIF(B:B,E57),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>127</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D58" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E58" s="0" t="str">
-        <f aca="false">IF(NOT(B58=B56),B58,"")</f>
+        <f aca="false">IF(NOT(B58=B57),B58,"")</f>
         <v/>
       </c>
       <c r="F58" s="0" t="str">
@@ -1993,42 +2043,42 @@
         <v/>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>129</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="false">IF(NOT(B59=B58),B59,"")</f>
-        <v/>
-      </c>
-      <c r="F59" s="0" t="str">
+        <v>Outlaw</v>
+      </c>
+      <c r="F59" s="0" t="n">
         <f aca="false">IF(NOT(E59=""),COUNTIF(B:B,E59),"")</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E60" s="0" t="str">
         <f aca="false">IF(NOT(B60=B59),B60,"")</f>
-        <v>Outlaw</v>
-      </c>
-      <c r="F60" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F60" s="0" t="str">
         <f aca="false">IF(NOT(E60=""),COUNTIF(B:B,E60),"")</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,7 +2086,7 @@
         <v>134</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>135</v>
@@ -2055,7 +2105,7 @@
         <v>136</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>137</v>
@@ -2069,14 +2119,14 @@
         <v/>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>138</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E63" s="0" t="str">
@@ -2088,51 +2138,75 @@
         <v/>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>140</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D64" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="0" t="str">
+        <f aca="false">IF(NOT(B64=B63),B64,"")</f>
+        <v/>
+      </c>
+      <c r="F64" s="0" t="str">
+        <f aca="false">IF(NOT(E64=""),COUNTIF(B:B,E64),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>142</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="0" t="str">
+        <f aca="false">IF(NOT(B65=B64),B65,"")</f>
+        <v/>
+      </c>
+      <c r="F65" s="0" t="str">
+        <f aca="false">IF(NOT(E65=""),COUNTIF(B:B,E65),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="0" t="str">
+        <f aca="false">IF(NOT(B66=B65),B66,"")</f>
+        <v/>
+      </c>
+      <c r="F66" s="0" t="str">
+        <f aca="false">IF(NOT(E66=""),COUNTIF(B:B,E66),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>146</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E67" s="0" t="str">
-        <f aca="false">IF(NOT(B67=B62),B67,"")</f>
+        <f aca="false">IF(NOT(B67=B66),B67,"")</f>
         <v/>
       </c>
       <c r="F67" s="0" t="str">
@@ -2140,14 +2214,14 @@
         <v/>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>148</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D68" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>149</v>
       </c>
       <c r="E68" s="0" t="str">
@@ -2164,7 +2238,7 @@
         <v>150</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>151</v>
@@ -2178,14 +2252,14 @@
         <v/>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>152</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D70" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E70" s="0" t="str">
@@ -2197,52 +2271,52 @@
         <v/>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>154</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="false">IF(NOT(B71=B70),B71,"")</f>
-        <v/>
-      </c>
-      <c r="F71" s="0" t="str">
+        <v>Scholar</v>
+      </c>
+      <c r="F71" s="0" t="n">
         <f aca="false">IF(NOT(E71=""),COUNTIF(B:B,E71),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>158</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="false">IF(NOT(B72=B71),B72,"")</f>
-        <v>Scholar</v>
-      </c>
-      <c r="F72" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F72" s="0" t="str">
         <f aca="false">IF(NOT(E72=""),COUNTIF(B:B,E72),"")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>159</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D73" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E73" s="0" t="str">
@@ -2254,12 +2328,12 @@
         <v/>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>161</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>162</v>
@@ -2278,7 +2352,7 @@
         <v>163</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>164</v>
@@ -2292,14 +2366,14 @@
         <v/>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>165</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D76" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>166</v>
       </c>
       <c r="E76" s="0" t="str">
@@ -2311,14 +2385,14 @@
         <v/>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>167</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>168</v>
       </c>
       <c r="E77" s="0" t="str">
@@ -2330,12 +2404,12 @@
         <v/>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>169</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>170</v>
@@ -2349,29 +2423,37 @@
         <v/>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>171</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D79" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="0" t="str">
+        <f aca="false">IF(NOT(B79=B78),B79,"")</f>
+        <v/>
+      </c>
+      <c r="F79" s="0" t="str">
+        <f aca="false">IF(NOT(E79=""),COUNTIF(B:B,E79),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>173</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>174</v>
       </c>
       <c r="E80" s="0" t="str">
-        <f aca="false">IF(NOT(B80=B78),B80,"")</f>
+        <f aca="false">IF(NOT(B80=B79),B80,"")</f>
         <v/>
       </c>
       <c r="F80" s="0" t="str">
@@ -2379,14 +2461,14 @@
         <v/>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>175</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D81" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>176</v>
       </c>
       <c r="E81" s="0" t="str">
@@ -2398,52 +2480,52 @@
         <v/>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>177</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="false">IF(NOT(B82=B81),B82,"")</f>
-        <v/>
-      </c>
-      <c r="F82" s="0" t="str">
+        <v>Sophisticate</v>
+      </c>
+      <c r="F82" s="0" t="n">
         <f aca="false">IF(NOT(E82=""),COUNTIF(B:B,E82),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D83" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="false">IF(NOT(B83=B82),B83,"")</f>
-        <v>Sophisticate</v>
-      </c>
-      <c r="F83" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F83" s="0" t="str">
         <f aca="false">IF(NOT(E83=""),COUNTIF(B:B,E83),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>182</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D84" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>183</v>
       </c>
       <c r="E84" s="0" t="str">
@@ -2455,14 +2537,14 @@
         <v/>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>184</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D85" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>185</v>
       </c>
       <c r="E85" s="0" t="str">
@@ -2474,12 +2556,12 @@
         <v/>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>186</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>187</v>
@@ -2493,14 +2575,14 @@
         <v/>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>188</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D87" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>189</v>
       </c>
       <c r="E87" s="0" t="str">
@@ -2512,12 +2594,12 @@
         <v/>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>190</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>191</v>
@@ -2531,12 +2613,12 @@
         <v/>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>192</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>193</v>
@@ -2550,12 +2632,12 @@
         <v/>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>194</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>195</v>
@@ -2569,12 +2651,12 @@
         <v/>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>196</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>197</v>
@@ -2593,7 +2675,7 @@
         <v>198</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>199</v>
@@ -2607,14 +2689,14 @@
         <v/>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>200</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>201</v>
       </c>
       <c r="E93" s="0" t="str">
@@ -2626,52 +2708,52 @@
         <v/>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>202</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D94" s="4" t="s">
         <v>203</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="false">IF(NOT(B94=B93),B94,"")</f>
-        <v/>
-      </c>
-      <c r="F94" s="0" t="str">
+        <v>Warrior</v>
+      </c>
+      <c r="F94" s="0" t="n">
         <f aca="false">IF(NOT(E94=""),COUNTIF(B:B,E94),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>206</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="false">IF(NOT(B95=B94),B95,"")</f>
-        <v>Warrior</v>
-      </c>
-      <c r="F95" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F95" s="0" t="str">
         <f aca="false">IF(NOT(E95=""),COUNTIF(B:B,E95),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>207</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D96" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>208</v>
       </c>
       <c r="E96" s="0" t="str">
@@ -2683,14 +2765,14 @@
         <v/>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>209</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D97" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>210</v>
       </c>
       <c r="E97" s="0" t="str">
@@ -2702,12 +2784,12 @@
         <v/>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>211</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>212</v>
@@ -2721,14 +2803,14 @@
         <v/>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>213</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D99" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>214</v>
       </c>
       <c r="E99" s="0" t="str">
@@ -2745,7 +2827,7 @@
         <v>215</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>216</v>
@@ -2759,14 +2841,14 @@
         <v/>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>217</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D101" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>218</v>
       </c>
       <c r="E101" s="0" t="str">
@@ -2778,12 +2860,12 @@
         <v/>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>219</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>220</v>
@@ -2797,12 +2879,12 @@
         <v/>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>221</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>222</v>
@@ -2821,7 +2903,7 @@
         <v>223</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>224</v>
@@ -2835,14 +2917,14 @@
         <v/>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>225</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D105" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>226</v>
       </c>
       <c r="E105" s="0" t="str">
@@ -2854,50 +2936,50 @@
         <v/>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>227</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D106" s="4" t="s">
         <v>228</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="false">IF(NOT(B106=B105),B106,"")</f>
-        <v/>
-      </c>
-      <c r="F106" s="0" t="str">
+        <v>Guru</v>
+      </c>
+      <c r="F106" s="0" t="n">
         <f aca="false">IF(NOT(E106=""),COUNTIF(B:B,E106),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>231</v>
       </c>
       <c r="E107" s="0" t="str">
         <f aca="false">IF(NOT(B107=B106),B107,"")</f>
-        <v>Guru</v>
-      </c>
-      <c r="F107" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F107" s="0" t="str">
         <f aca="false">IF(NOT(E107=""),COUNTIF(B:B,E107),"")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>232</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>233</v>
@@ -2911,12 +2993,12 @@
         <v/>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>234</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>235</v>
@@ -2930,12 +3012,12 @@
         <v/>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>236</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>237</v>
@@ -2949,12 +3031,12 @@
         <v/>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>238</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>239</v>
@@ -2968,12 +3050,12 @@
         <v/>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>240</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>241</v>
@@ -2987,12 +3069,12 @@
         <v/>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>242</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>243</v>
@@ -3006,12 +3088,12 @@
         <v/>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>244</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>245</v>
@@ -3025,12 +3107,12 @@
         <v/>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>246</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>247</v>
@@ -3049,25 +3131,22 @@
         <v>248</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B117" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>251</v>
+      <c r="E116" s="0" t="str">
+        <f aca="false">IF(NOT(B116=B115),B116,"")</f>
+        <v/>
+      </c>
+      <c r="F116" s="0" t="str">
+        <f aca="false">IF(NOT(E116=""),COUNTIF(B:B,E116),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D94"/>
+  <autoFilter ref="A1:D105"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Languages added + linguistics skill modified from technology
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Feats/Feats.xlsx
+++ b/CoreRulebook/Data/Feats/Feats.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$125</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$113</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$D$98</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$112</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$124</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$100</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$D$97</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="267">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">Crash Course</t>
   </si>
   <si>
-    <t xml:space="preserve">You study a crash course in a selection of 10 abilities you previously had no skill in, giving you a basic level of knowledge. Choose up to 10 \imp{Abilities} with a \emptyCape{} rating, and gain 1 dot in each of them. If, when you take this ability, it would cost more than 9 dots, pay only 9 dots. </t>
+    <t xml:space="preserve">You study a crash course in a selection of 10 abilities you previously had no skill in, giving you a basic level of knowledge. Choose up to 10 \imp{Abilities} with a \emptyCape{} rating, and gain 1 dot in each of them. </t>
   </si>
   <si>
     <t xml:space="preserve">Elemental Attunement</t>
@@ -91,7 +91,7 @@
   <si>
     <t xml:space="preserve">As a witch or wizard, the chaotic force of magic flows within your veins. You have learned to harness this magic in some innate way beyond the usual spellcasting. This effect is usually minor (something a Muggle could put down to an act of trickery or showmanship), and often forms the basis of a parlour trick. 
 You might be able to summon a small flame from your finger, make your eyes into burning coals or deep black voids, play a stirring soundtrack whenever they engage in a fight, know the name of every individual you meet, or some other marvellous but ultimately slightly inconsequential feat that you could imagine being the focus of conversation at a party. 
-No rolls are needed to use this ability, and the GM has a veto if this tool is being used in an inappropriate fashion. {\bf This ability costs half the usual amount for a feat.}</t>
+No rolls are needed to use this ability, and the GM has a veto if this tool is being used in an inappropriate fashion. {\bf This ability costs only 4 \imp{EXP}.}</t>
   </si>
   <si>
     <t xml:space="preserve">Instinctive Defence</t>
@@ -111,12 +111,6 @@
   </si>
   <si>
     <t xml:space="preserve">You need much less sleep than others, and can go from asleep to awake in a blink of an eye. You gain the benefits of a \imp{Long Rest} after only 4 hours, and may ignore the effects of \imp{Level One Exhaustion}. Any \imp{Alertness} checks called for whilst asleep have the DV reduced by 3.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linguist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have studied another language enough to be considered fluent in it. When conversing in this language, gain +2d to all social checks. You may take this ability multiple times, learning a new language each time. </t>
   </si>
   <si>
     <t xml:space="preserve">Loyal Companion</t>
@@ -971,10 +965,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1019,7 +1013,7 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">IF(NOT(E2=""),COUNTIF(B:B,E2),"")</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1035,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1120,7 +1114,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="136.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
@@ -1196,37 +1190,40 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="0" t="str">
-        <f aca="false">IF(NOT(B12=B11),B12,"")</f>
-        <v/>
-      </c>
-      <c r="F12" s="0" t="str">
+        <v>29</v>
+      </c>
+      <c r="E12" s="0" t="e">
+        <f aca="false">IF(NOT(B12=#REF!),B12,"")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F12" s="0" t="e">
         <f aca="false">IF(NOT(E12=""),COUNTIF(B:B,E12),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="0" t="str">
         <f aca="false">IF(NOT(B13=B12),B13,"")</f>
@@ -1237,15 +1234,12 @@
         <v/>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>34</v>
@@ -1266,8 +1260,11 @@
       <c r="B15" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="0" t="str">
         <f aca="false">IF(NOT(B15=B14),B15,"")</f>
@@ -1278,16 +1275,13 @@
         <v/>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1300,15 +1294,18 @@
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C17" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="0" t="str">
         <f aca="false">IF(NOT(B17=B16),B17,"")</f>
@@ -1319,18 +1316,18 @@
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="false">IF(NOT(B18=B17),B18,"")</f>
@@ -1341,16 +1338,13 @@
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
@@ -1363,7 +1357,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>48</v>
       </c>
@@ -1382,7 +1376,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>50</v>
       </c>
@@ -1401,13 +1395,16 @@
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C22" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1420,53 +1417,50 @@
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E23" s="0" t="str">
         <f aca="false">IF(NOT(B23=B22),B23,"")</f>
-        <v/>
-      </c>
-      <c r="F23" s="0" t="str">
+        <v>Artificer</v>
+      </c>
+      <c r="F23" s="0" t="n">
         <f aca="false">IF(NOT(E23=""),COUNTIF(B:B,E23),"")</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E24" s="0" t="str">
         <f aca="false">IF(NOT(B24=B23),B24,"")</f>
-        <v>Artificer</v>
-      </c>
-      <c r="F24" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F24" s="0" t="str">
         <f aca="false">IF(NOT(E24=""),COUNTIF(B:B,E24),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>59</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>60</v>
@@ -1480,12 +1474,12 @@
         <v/>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>62</v>
@@ -1499,12 +1493,12 @@
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>64</v>
@@ -1518,12 +1512,12 @@
         <v/>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>66</v>
@@ -1537,12 +1531,12 @@
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>67</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>68</v>
@@ -1561,7 +1555,7 @@
         <v>69</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>70</v>
@@ -1575,12 +1569,12 @@
         <v/>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>71</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>72</v>
@@ -1599,7 +1593,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>74</v>
@@ -1613,12 +1607,12 @@
         <v/>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>75</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>76</v>
@@ -1632,12 +1626,12 @@
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>78</v>
@@ -1651,50 +1645,50 @@
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>79</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E35" s="0" t="str">
         <f aca="false">IF(NOT(B35=B34),B35,"")</f>
-        <v/>
-      </c>
-      <c r="F35" s="0" t="str">
+        <v>Auror</v>
+      </c>
+      <c r="F35" s="0" t="n">
         <f aca="false">IF(NOT(E35=""),COUNTIF(B:B,E35),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E36" s="0" t="str">
         <f aca="false">IF(NOT(B36=B35),B36,"")</f>
-        <v>Auror</v>
-      </c>
-      <c r="F36" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F36" s="0" t="str">
         <f aca="false">IF(NOT(E36=""),COUNTIF(B:B,E36),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>85</v>
@@ -1708,14 +1702,14 @@
         <v/>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>86</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E38" s="0" t="str">
@@ -1727,14 +1721,14 @@
         <v/>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E39" s="0" t="str">
@@ -1746,14 +1740,14 @@
         <v/>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>90</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E40" s="0" t="str">
@@ -1770,7 +1764,7 @@
         <v>92</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>93</v>
@@ -1784,14 +1778,14 @@
         <v/>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>94</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E42" s="0" t="str">
@@ -1803,14 +1797,14 @@
         <v/>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>96</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>97</v>
       </c>
       <c r="E43" s="0" t="str">
@@ -1822,14 +1816,14 @@
         <v/>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>98</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E44" s="0" t="str">
@@ -1841,14 +1835,14 @@
         <v/>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>100</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>101</v>
       </c>
       <c r="E45" s="0" t="str">
@@ -1860,12 +1854,12 @@
         <v/>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>102</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>103</v>
@@ -1879,50 +1873,50 @@
         <v/>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>104</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="false">IF(NOT(B47=B46),B47,"")</f>
-        <v/>
-      </c>
-      <c r="F47" s="0" t="str">
+        <v>Druid</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <f aca="false">IF(NOT(E47=""),COUNTIF(B:B,E47),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>108</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="false">IF(NOT(B48=B47),B48,"")</f>
-        <v>Druid</v>
-      </c>
-      <c r="F48" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F48" s="0" t="str">
         <f aca="false">IF(NOT(E48=""),COUNTIF(B:B,E48),"")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>109</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>110</v>
@@ -1936,12 +1930,12 @@
         <v/>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>111</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>112</v>
@@ -1955,12 +1949,12 @@
         <v/>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>113</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>114</v>
@@ -1974,12 +1968,12 @@
         <v/>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>115</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>116</v>
@@ -1998,7 +1992,7 @@
         <v>117</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>118</v>
@@ -2012,12 +2006,12 @@
         <v/>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>120</v>
@@ -2031,14 +2025,14 @@
         <v/>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>121</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>122</v>
       </c>
       <c r="E55" s="0" t="str">
@@ -2050,12 +2044,12 @@
         <v/>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>123</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>124</v>
@@ -2069,14 +2063,14 @@
         <v/>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>125</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D57" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E57" s="0" t="str">
@@ -2088,50 +2082,50 @@
         <v/>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>127</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E58" s="0" t="str">
         <f aca="false">IF(NOT(B58=B57),B58,"")</f>
-        <v/>
-      </c>
-      <c r="F58" s="0" t="str">
+        <v>Guru</v>
+      </c>
+      <c r="F58" s="0" t="n">
         <f aca="false">IF(NOT(E58=""),COUNTIF(B:B,E58),"")</f>
-        <v/>
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>131</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="false">IF(NOT(B59=B58),B59,"")</f>
-        <v>Guru</v>
-      </c>
-      <c r="F59" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F59" s="0" t="str">
         <f aca="false">IF(NOT(E59=""),COUNTIF(B:B,E59),"")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>132</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>133</v>
@@ -2150,7 +2144,7 @@
         <v>134</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>135</v>
@@ -2164,12 +2158,12 @@
         <v/>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>136</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>137</v>
@@ -2183,12 +2177,12 @@
         <v/>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>138</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>139</v>
@@ -2202,12 +2196,12 @@
         <v/>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>140</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>141</v>
@@ -2221,12 +2215,12 @@
         <v/>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>142</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>143</v>
@@ -2240,12 +2234,12 @@
         <v/>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>145</v>
@@ -2259,12 +2253,12 @@
         <v/>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>146</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>147</v>
@@ -2278,12 +2272,12 @@
         <v/>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>148</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>149</v>
@@ -2297,42 +2291,42 @@
         <v/>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>150</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E69" s="0" t="str">
         <f aca="false">IF(NOT(B69=B68),B69,"")</f>
-        <v/>
-      </c>
-      <c r="F69" s="0" t="str">
+        <v>Outlaw</v>
+      </c>
+      <c r="F69" s="0" t="n">
         <f aca="false">IF(NOT(E69=""),COUNTIF(B:B,E69),"")</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E70" s="0" t="str">
         <f aca="false">IF(NOT(B70=B69),B70,"")</f>
-        <v>Outlaw</v>
-      </c>
-      <c r="F70" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F70" s="0" t="str">
         <f aca="false">IF(NOT(E70=""),COUNTIF(B:B,E70),"")</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2334,7 @@
         <v>155</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>156</v>
@@ -2359,7 +2353,7 @@
         <v>157</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>158</v>
@@ -2373,14 +2367,14 @@
         <v/>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>159</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E73" s="0" t="str">
@@ -2392,14 +2386,14 @@
         <v/>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>161</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>162</v>
       </c>
       <c r="E74" s="0" t="str">
@@ -2411,14 +2405,14 @@
         <v/>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>163</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D75" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>164</v>
       </c>
       <c r="E75" s="0" t="str">
@@ -2430,12 +2424,12 @@
         <v/>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>165</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>166</v>
@@ -2449,14 +2443,14 @@
         <v/>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>167</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D77" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>168</v>
       </c>
       <c r="E77" s="0" t="str">
@@ -2468,14 +2462,14 @@
         <v/>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>169</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D78" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>170</v>
       </c>
       <c r="E78" s="0" t="str">
@@ -2492,7 +2486,7 @@
         <v>171</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>172</v>
@@ -2506,14 +2500,14 @@
         <v/>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>173</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D80" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E80" s="0" t="str">
@@ -2525,61 +2519,53 @@
         <v/>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>175</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E81" s="0" t="str">
         <f aca="false">IF(NOT(B81=B80),B81,"")</f>
-        <v/>
-      </c>
-      <c r="F81" s="0" t="str">
+        <v>Responder</v>
+      </c>
+      <c r="F81" s="0" t="n">
         <f aca="false">IF(NOT(E81=""),COUNTIF(B:B,E81),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="false">IF(NOT(B82=B81),B82,"")</f>
-        <v>Responder</v>
-      </c>
-      <c r="F82" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F82" s="0" t="str">
         <f aca="false">IF(NOT(E82=""),COUNTIF(B:B,E82),"")</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>180</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E83" s="0" t="str">
-        <f aca="false">IF(NOT(B83=B82),B83,"")</f>
-        <v/>
-      </c>
-      <c r="F83" s="0" t="str">
-        <f aca="false">IF(NOT(E83=""),COUNTIF(B:B,E83),"")</f>
-        <v/>
       </c>
     </row>
     <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,40 +2573,40 @@
         <v>182</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>184</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="125.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>186</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="125.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>188</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>189</v>
@@ -2631,70 +2617,78 @@
         <v>190</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>192</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>194</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>196</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="D91" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D91" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E91" s="0" t="str">
+        <f aca="false">IF(NOT(B91=B82),B91,"")</f>
+        <v>Scholar</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <f aca="false">IF(NOT(E91=""),COUNTIF(B:B,E91),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D92" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>200</v>
       </c>
       <c r="E92" s="0" t="str">
-        <f aca="false">IF(NOT(B92=B83),B92,"")</f>
-        <v>Scholar</v>
-      </c>
-      <c r="F92" s="0" t="n">
+        <f aca="false">IF(NOT(B92=B91),B92,"")</f>
+        <v/>
+      </c>
+      <c r="F92" s="0" t="str">
         <f aca="false">IF(NOT(E92=""),COUNTIF(B:B,E92),"")</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>201</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>202</v>
@@ -2713,7 +2707,7 @@
         <v>203</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>204</v>
@@ -2727,14 +2721,14 @@
         <v/>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>205</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D95" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>206</v>
       </c>
       <c r="E95" s="0" t="str">
@@ -2746,14 +2740,14 @@
         <v/>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>207</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D96" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>208</v>
       </c>
       <c r="E96" s="0" t="str">
@@ -2765,14 +2759,14 @@
         <v/>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>209</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D97" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>210</v>
       </c>
       <c r="E97" s="0" t="str">
@@ -2784,12 +2778,12 @@
         <v/>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>211</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>212</v>
@@ -2808,7 +2802,7 @@
         <v>213</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>214</v>
@@ -2822,14 +2816,14 @@
         <v/>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>215</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D100" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>216</v>
       </c>
       <c r="E100" s="0" t="str">
@@ -2841,52 +2835,52 @@
         <v/>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>217</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="false">IF(NOT(B101=B100),B101,"")</f>
-        <v/>
-      </c>
-      <c r="F101" s="0" t="str">
+        <v>Sophisticate</v>
+      </c>
+      <c r="F101" s="0" t="n">
         <f aca="false">IF(NOT(E101=""),COUNTIF(B:B,E101),"")</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>221</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="false">IF(NOT(B102=B101),B102,"")</f>
-        <v>Sophisticate</v>
-      </c>
-      <c r="F102" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F102" s="0" t="str">
         <f aca="false">IF(NOT(E102=""),COUNTIF(B:B,E102),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>222</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D103" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>223</v>
       </c>
       <c r="E103" s="0" t="str">
@@ -2898,14 +2892,14 @@
         <v/>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>224</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D104" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E104" s="0" t="str">
@@ -2917,14 +2911,14 @@
         <v/>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>226</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D105" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>227</v>
       </c>
       <c r="E105" s="0" t="str">
@@ -2936,12 +2930,12 @@
         <v/>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>228</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>229</v>
@@ -2955,14 +2949,14 @@
         <v/>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>230</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D107" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>231</v>
       </c>
       <c r="E107" s="0" t="str">
@@ -2974,12 +2968,12 @@
         <v/>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>232</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>233</v>
@@ -2993,12 +2987,12 @@
         <v/>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>234</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>235</v>
@@ -3012,12 +3006,12 @@
         <v/>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>236</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>237</v>
@@ -3031,12 +3025,12 @@
         <v/>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>238</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>239</v>
@@ -3050,14 +3044,14 @@
         <v/>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>240</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D112" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D112" s="4" t="s">
         <v>241</v>
       </c>
       <c r="E112" s="0" t="str">
@@ -3069,52 +3063,52 @@
         <v/>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>242</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D113" s="4" t="s">
         <v>243</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="E113" s="0" t="str">
         <f aca="false">IF(NOT(B113=B112),B113,"")</f>
-        <v/>
-      </c>
-      <c r="F113" s="0" t="str">
+        <v>Warrior</v>
+      </c>
+      <c r="F113" s="0" t="n">
         <f aca="false">IF(NOT(E113=""),COUNTIF(B:B,E113),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>246</v>
       </c>
       <c r="E114" s="0" t="str">
         <f aca="false">IF(NOT(B114=B113),B114,"")</f>
-        <v>Warrior</v>
-      </c>
-      <c r="F114" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F114" s="0" t="str">
         <f aca="false">IF(NOT(E114=""),COUNTIF(B:B,E114),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>247</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D115" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D115" s="4" t="s">
         <v>248</v>
       </c>
       <c r="E115" s="0" t="str">
@@ -3126,14 +3120,14 @@
         <v/>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>249</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D116" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>250</v>
       </c>
       <c r="E116" s="0" t="str">
@@ -3145,12 +3139,12 @@
         <v/>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>251</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>252</v>
@@ -3164,14 +3158,14 @@
         <v/>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>253</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D118" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D118" s="4" t="s">
         <v>254</v>
       </c>
       <c r="E118" s="0" t="str">
@@ -3188,7 +3182,7 @@
         <v>255</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>256</v>
@@ -3202,14 +3196,14 @@
         <v/>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>257</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D120" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>258</v>
       </c>
       <c r="E120" s="0" t="str">
@@ -3221,12 +3215,12 @@
         <v/>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>259</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>260</v>
@@ -3240,12 +3234,12 @@
         <v/>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>261</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>262</v>
@@ -3264,7 +3258,7 @@
         <v>263</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>264</v>
@@ -3278,14 +3272,14 @@
         <v/>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>265</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D124" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D124" s="4" t="s">
         <v>266</v>
       </c>
       <c r="E124" s="0" t="str">
@@ -3297,47 +3291,28 @@
         <v/>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B125" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="E125" s="0" t="str">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E125" s="0" t="n">
         <f aca="false">IF(NOT(B125=B124),B125,"")</f>
-        <v/>
-      </c>
-      <c r="F125" s="0" t="str">
+        <v>0</v>
+      </c>
+      <c r="F125" s="0" t="n">
         <f aca="false">IF(NOT(E125=""),COUNTIF(B:B,E125),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E126" s="0" t="n">
+      <c r="E126" s="0" t="str">
         <f aca="false">IF(NOT(B126=B125),B126,"")</f>
-        <v>0</v>
-      </c>
-      <c r="F126" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F126" s="0" t="str">
         <f aca="false">IF(NOT(E126=""),COUNTIF(B:B,E126),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E127" s="0" t="str">
-        <f aca="false">IF(NOT(B127=B126),B127,"")</f>
-        <v/>
-      </c>
-      <c r="F127" s="0" t="str">
-        <f aca="false">IF(NOT(E127=""),COUNTIF(B:B,E127),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D125"/>
+  <autoFilter ref="A1:D112"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Changes to character sheet + major/minor actions
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Feats/Feats.xlsx
+++ b/CoreRulebook/Data/Feats/Feats.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$121</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$D$109</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$122</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$D$110</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$98</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$D$95</definedName>
   </definedNames>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="263">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -442,23 +442,7 @@
     <t xml:space="preserve">Self Improvement</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Whenever you cast a spell with a range of \imp{Self}, gain one additional auto-success. In addition, a number of times per day equal to your \imp{Self} rating, w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">hen you cast a spell with a range of \imp{Self} which would impact your combat ability, you may immediately take a melee attack on a foe in range. </t>
-    </r>
+    <t xml:space="preserve">Whenever you cast a spell with a range of \imp{Self}, gain one additional auto-success. In addition, a number of times per day equal to your \imp{Self} rating, when you cast a spell with a range of \imp{Self} which would impact your combat ability, you may immediately take a melee attack on a foe in range. </t>
   </si>
   <si>
     <t xml:space="preserve">Silent Step</t>
@@ -533,23 +517,7 @@
     <t xml:space="preserve">Naturally Shifty</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Doing unscrupulous deeds comes as naturally to you as breathing – gain one additional auto-success on any \imp{Covert} action. In addition, w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">hilst you are outside of bright light, all \imp{Covert} actions have a DV one lower than normal.</t>
-    </r>
+    <t xml:space="preserve">Doing unscrupulous deeds comes as naturally to you as breathing – gain one additional auto-success on any \imp{Covert} action. In addition, whilst you are outside of bright light, all \imp{Covert} actions have a DV one lower than normal.</t>
   </si>
   <si>
     <t xml:space="preserve">Play the System</t>
@@ -659,7 +627,7 @@
     <t xml:space="preserve">Learn From Failure</t>
   </si>
   <si>
-    <t xml:space="preserve">When performing a check of any kind, for every consectutive previous roll (of any kind) failed by you or your allies, you gain +1d (up to a maximum of your \imp{Stubbornness} rating).</t>
+    <t xml:space="preserve">When performing a check of any kind, for every consecutive previous roll (of any kind) failed by you or your allies, you gain +1d (up to a maximum of your \imp{Stubbornness} rating).</t>
   </si>
   <si>
     <t xml:space="preserve">Library Lover</t>
@@ -695,29 +663,13 @@
     <t xml:space="preserve">Absorb Information</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">You have a near-eidetic memory, and can accurately recall any information you have seen, read, or heard about in the past 24 hours. In addition, y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ou need to spend half the usual time in order to learn a new spell, or memorise an enchanting rune, and automatically succeed on the final memorisation roll for spells.</t>
-    </r>
+    <t xml:space="preserve">You have a near-eidetic memory, and can accurately recall any information you have seen, read, or heard about in the past 24 hours. In addition, you need to spend half the usual time in order to learn a new spell, or memorise an enchanting rune, and automatically succeed on the final memorisation roll for spells.</t>
   </si>
   <si>
     <t xml:space="preserve">Subject Expertise</t>
   </si>
   <si>
-    <t xml:space="preserve">Choose a spell discipline, a type of creature, or another kind of action or area of knowledge: you are considered an up-and-coming expert in this field. When performing a check of any kind to target the subjetc of your knowledge, use the associated skills (such as a spellcasting check) or to research more information about the subject of your expertise, you gain one additional auto-success. 
+    <t xml:space="preserve">Choose a spell discipline, a type of creature, or another kind of action or area of knowledge: you are considered an up-and-coming expert in this field. When performing a check of any kind to target the subject of your knowledge, use the associated skills (such as a spellcasting check) or to research more information about the subject of your expertise, you gain one additional auto-success. 
 During a prolonged period of \imp{Downtime}, you may shift your choice of expertise to any other field. </t>
   </si>
   <si>
@@ -745,7 +697,7 @@
     <t xml:space="preserve">Charmed Life</t>
   </si>
   <si>
-    <t xml:space="preserve">A number of times per day equal to your \imp{Wealth} rating, you can negate the negative consequences of a \imp{Catastrophic} failure suffered by you or your allies, or grant a +1d bonus on any check that you can see occuring. </t>
+    <t xml:space="preserve">A number of times per day equal to your \imp{Wealth} rating, you can negate the negative consequences of a \imp{Catastrophic} failure suffered by you or your allies, or grant a +1d bonus on any check that you can see occurring. </t>
   </si>
   <si>
     <t xml:space="preserve">Distracting Shout</t>
@@ -754,6 +706,12 @@
     <t xml:space="preserve">Your forceful presence extends onto the battlefield – whilst in combat you can use a \imp{minor action} to select a target which has not yet declared their action within 10m and perform some action to get their attention. You may either force them to focus all attacks on you this turn, {\bf or} distract them, imposing a 1d penalty on any action they take. </t>
   </si>
   <si>
+    <t xml:space="preserve">Eyes on the Prize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever you perform a \imp{Major Action} which requires a roll, you may take a 1d penalty to \imp{Take Stock} as an instantaneous action. You also gain +1d to counteract acts of sleight-of-hand and other such chicanery. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Magical Conversation</t>
   </si>
   <si>
@@ -850,7 +808,7 @@
     <t xml:space="preserve">Mind over Matter</t>
   </si>
   <si>
-    <t xml:space="preserve">You may \imp{Endure} the harm caused by physical \imp{harm}. Whilst your \imp{Endure} rating remains above zero, dice penalties due to \imp{Harm} are one level less serious.</t>
+    <t xml:space="preserve">You may \imp{Endure} the damage caused by physical \imp{harm}. Whilst your \imp{Endure} rating remains above zero, dice penalties due to \imp{Harm} are one level less serious.</t>
   </si>
   <si>
     <t xml:space="preserve">Never Give In</t>
@@ -878,7 +836,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -905,16 +863,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -959,7 +907,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -980,18 +928,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1001,23 +945,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="77.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2795,7 +2738,7 @@
       <c r="B96" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="4" t="s">
         <v>208</v>
       </c>
       <c r="E96" s="0" t="str">
@@ -2807,7 +2750,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="56.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>209</v>
       </c>
@@ -2861,7 +2804,7 @@
       </c>
       <c r="F99" s="0" t="n">
         <f aca="false">IF(NOT(E99=""),COUNTIF(B:B,E99),"")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2913,26 +2856,18 @@
         <v/>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>222</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E103" s="0" t="str">
-        <f aca="false">IF(NOT(B103=B102),B103,"")</f>
-        <v/>
-      </c>
-      <c r="F103" s="0" t="str">
-        <f aca="false">IF(NOT(E103=""),COUNTIF(B:B,E103),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="104" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>224</v>
       </c>
@@ -2943,7 +2878,7 @@
         <v>225</v>
       </c>
       <c r="E104" s="0" t="str">
-        <f aca="false">IF(NOT(B104=B103),B104,"")</f>
+        <f aca="false">IF(NOT(B104=B102),B104,"")</f>
         <v/>
       </c>
       <c r="F104" s="0" t="str">
@@ -2951,14 +2886,14 @@
         <v/>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>226</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="4" t="s">
         <v>227</v>
       </c>
       <c r="E105" s="0" t="str">
@@ -2970,7 +2905,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>228</v>
       </c>
@@ -2989,7 +2924,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>230</v>
       </c>
@@ -3027,14 +2962,14 @@
         <v/>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>234</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="1" t="s">
         <v>235</v>
       </c>
       <c r="E109" s="0" t="str">
@@ -3046,50 +2981,50 @@
         <v/>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>236</v>
       </c>
       <c r="B110" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="D110" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="E110" s="0" t="str">
         <f aca="false">IF(NOT(B110=B109),B110,"")</f>
-        <v>Warrior</v>
-      </c>
-      <c r="F110" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F110" s="0" t="str">
         <f aca="false">IF(NOT(E110=""),COUNTIF(B:B,E110),"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v/>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B111" s="0" t="s">
         <v>239</v>
-      </c>
-      <c r="B111" s="0" t="s">
-        <v>237</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>240</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="false">IF(NOT(B111=B110),B111,"")</f>
-        <v/>
-      </c>
-      <c r="F111" s="0" t="str">
+        <v>Warrior</v>
+      </c>
+      <c r="F111" s="0" t="n">
         <f aca="false">IF(NOT(E111=""),COUNTIF(B:B,E111),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>241</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>242</v>
@@ -3103,12 +3038,12 @@
         <v/>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>243</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>244</v>
@@ -3122,48 +3057,48 @@
         <v/>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>245</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="115" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E114" s="0" t="str">
+        <f aca="false">IF(NOT(B114=B113),B114,"")</f>
+        <v/>
+      </c>
+      <c r="F114" s="0" t="str">
+        <f aca="false">IF(NOT(E114=""),COUNTIF(B:B,E114),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>247</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D115" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E115" s="0" t="str">
-        <f aca="false">IF(NOT(B115=B113),B115,"")</f>
-        <v/>
-      </c>
-      <c r="F115" s="0" t="str">
-        <f aca="false">IF(NOT(E115=""),COUNTIF(B:B,E115),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="116" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>249</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>250</v>
       </c>
       <c r="E116" s="0" t="str">
-        <f aca="false">IF(NOT(B116=B115),B116,"")</f>
+        <f aca="false">IF(NOT(B116=B114),B116,"")</f>
         <v/>
       </c>
       <c r="F116" s="0" t="str">
@@ -3171,14 +3106,14 @@
         <v/>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>251</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D117" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D117" s="4" t="s">
         <v>252</v>
       </c>
       <c r="E117" s="0" t="str">
@@ -3190,12 +3125,12 @@
         <v/>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>253</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>254</v>
@@ -3209,12 +3144,12 @@
         <v/>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>255</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>256</v>
@@ -3233,7 +3168,7 @@
         <v>257</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>258</v>
@@ -3247,14 +3182,14 @@
         <v/>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>259</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D121" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>260</v>
       </c>
       <c r="E121" s="0" t="str">
@@ -3266,10 +3201,19 @@
         <v/>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E122" s="0" t="n">
+    <row r="122" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E122" s="0" t="str">
         <f aca="false">IF(NOT(B122=B121),B122,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="F122" s="0" t="str">
         <f aca="false">IF(NOT(E122=""),COUNTIF(B:B,E122),"")</f>
@@ -3277,13 +3221,13 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E123" s="0" t="str">
+      <c r="E123" s="0" t="n">
         <f aca="false">IF(NOT(B123=B122),B123,"")</f>
-        <v/>
-      </c>
-      <c r="F123" s="0" t="str">
+        <v>0</v>
+      </c>
+      <c r="F123" s="0" t="n">
         <f aca="false">IF(NOT(E123=""),COUNTIF(B:B,E123),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,8 +3240,18 @@
         <v/>
       </c>
     </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E125" s="0" t="str">
+        <f aca="false">IF(NOT(B125=B124),B125,"")</f>
+        <v/>
+      </c>
+      <c r="F125" s="0" t="str">
+        <f aca="false">IF(NOT(E125=""),COUNTIF(B:B,E125),"")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D121"/>
+  <autoFilter ref="A1:D122"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>